<commit_message>
Updated Decoder module to reflect new ISA and readme
</commit_message>
<xml_diff>
--- a/docs/8bit_CPU_Instruction_Set.xlsx
+++ b/docs/8bit_CPU_Instruction_Set.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adria\Desktop\8Bit_CPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8EDD70-E154-4910-B8EF-B9A9CCEB4F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD904E26-4CF5-4363-A544-3C7E168A3AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
   <si>
     <t>Category</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Branch / Control</t>
   </si>
   <si>
-    <t>Jump / Link</t>
-  </si>
-  <si>
     <t>add</t>
   </si>
   <si>
@@ -79,12 +76,6 @@
     <t>sra</t>
   </si>
   <si>
-    <t>lb</t>
-  </si>
-  <si>
-    <t>sb</t>
-  </si>
-  <si>
     <t>beq</t>
   </si>
   <si>
@@ -97,9 +88,6 @@
     <t>jump</t>
   </si>
   <si>
-    <t>jal</t>
-  </si>
-  <si>
     <t>add R1,R2,R3</t>
   </si>
   <si>
@@ -130,9 +118,6 @@
     <t>sra R1,R2</t>
   </si>
   <si>
-    <t>lb R1,5(R2)</t>
-  </si>
-  <si>
     <t>sb R1,5(R2)</t>
   </si>
   <si>
@@ -148,9 +133,6 @@
     <t>jump label</t>
   </si>
   <si>
-    <t>jal label</t>
-  </si>
-  <si>
     <t>R1 = R2 + R3</t>
   </si>
   <si>
@@ -199,9 +181,6 @@
     <t>PC = label</t>
   </si>
   <si>
-    <t>R7 = PC + 2; PC = label</t>
-  </si>
-  <si>
     <t>3 registers; basic addition</t>
   </si>
   <si>
@@ -232,12 +211,6 @@
     <t>Shift right arithmetic</t>
   </si>
   <si>
-    <t>Load byte from memory</t>
-  </si>
-  <si>
-    <t>Store byte to memory</t>
-  </si>
-  <si>
     <t>Branch if equal</t>
   </si>
   <si>
@@ -248,9 +221,6 @@
   </si>
   <si>
     <t>Unconditional jump</t>
-  </si>
-  <si>
-    <t>Jump and link (function call)</t>
   </si>
   <si>
     <t xml:space="preserve">    Arithmetic</t>
@@ -444,12 +414,54 @@
       <t>: offset for load/store instructions</t>
     </r>
   </si>
+  <si>
+    <t>2-0</t>
+  </si>
+  <si>
+    <t>8-6</t>
+  </si>
+  <si>
+    <t>bit indices</t>
+  </si>
+  <si>
+    <t>5-3</t>
+  </si>
+  <si>
+    <t>11-9</t>
+  </si>
+  <si>
+    <t>15-12</t>
+  </si>
+  <si>
+    <t>lw</t>
+  </si>
+  <si>
+    <t>lw R1,5(R2)</t>
+  </si>
+  <si>
+    <t>HLT</t>
+  </si>
+  <si>
+    <t>Terminate program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump </t>
+  </si>
+  <si>
+    <t>sw</t>
+  </si>
+  <si>
+    <t>Store word to memory</t>
+  </si>
+  <si>
+    <t>Load word from memory</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,6 +502,12 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -566,6 +584,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -575,16 +594,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -905,7 +921,7 @@
     <col min="6" max="8" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -922,437 +938,454 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" t="s">
         <v>78</v>
       </c>
-      <c r="I1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J1" t="s">
-        <v>88</v>
-      </c>
       <c r="K1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="L1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="M1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="6"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A3" s="7"/>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="3" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>93</v>
-      </c>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="6"/>
+    <row r="4" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A4" s="7"/>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="I5" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K5" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="L5" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-    </row>
-    <row r="5" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A5" s="6"/>
-      <c r="B5" s="3" t="s">
+      <c r="M5" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A6" s="7"/>
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="I6" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A7" s="7"/>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="I7" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="I8" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A9" s="8"/>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="I9" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A10" s="8"/>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="I10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A11" s="8"/>
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="I11" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A13" s="8"/>
+      <c r="B13" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="6"/>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="F14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A15" s="8"/>
+      <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="I6" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A7" s="6"/>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="F15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A16" s="8"/>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="I7" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="F16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="A17" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="I8" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A9" s="7"/>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="I9" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A10" s="7"/>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="I10" s="11" t="s">
+      <c r="F17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="A18" s="8"/>
+      <c r="B18" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="J10" s="11"/>
-    </row>
-    <row r="11" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A11" s="7"/>
-      <c r="B11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="I11" s="11" t="s">
+      <c r="C18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A12" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A13" s="7"/>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A15" s="7"/>
-      <c r="B15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A16" s="7"/>
-      <c r="B16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="A17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="A18" s="7"/>
-      <c r="B18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="F18" s="3"/>
       <c r="G18" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="J4:M4"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A17:A18"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="J4:M4"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>